<commit_message>
Work on alu, alu control and control unit
</commit_message>
<xml_diff>
--- a/ISA/ISA.xlsx
+++ b/ISA/ISA.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emari\Desktop\Proyecto-Grupal-1---Arqui-I\ISA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972AB32E-86DA-4D16-A160-4410CE4058B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD1C1E0-4EC9-4366-BFB3-C65BDF09A533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C6F3682-6770-4276-A143-9EE1D7FB331A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8C6F3682-6770-4276-A143-9EE1D7FB331A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="178">
   <si>
     <t>load byte</t>
   </si>
@@ -189,9 +190,6 @@
     <t>funct2</t>
   </si>
   <si>
-    <t>func2</t>
-  </si>
-  <si>
     <t>rd</t>
   </si>
   <si>
@@ -511,6 +509,69 @@
   </si>
   <si>
     <t>Jump to the instruction labeled by dir if previous comparison is less than.</t>
+  </si>
+  <si>
+    <t>ALUOp</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>load register</t>
+  </si>
+  <si>
+    <t>store register</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>sub</t>
+  </si>
+  <si>
+    <t>mul</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>shift left</t>
+  </si>
+  <si>
+    <t>shift right</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>ALU Control</t>
   </si>
 </sst>
 </file>
@@ -733,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -757,6 +818,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -775,6 +845,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -784,6 +872,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -793,45 +890,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1168,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48BD489-9536-4BB1-9C3B-2CF1BDBFC0B2}">
   <dimension ref="B1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -1186,378 +1254,378 @@
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="2:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
@@ -1567,19 +1635,19 @@
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1587,22 +1655,22 @@
         <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1610,22 +1678,22 @@
         <v>10</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1671,7 +1739,7 @@
   <dimension ref="A5:AJ34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1684,49 +1752,49 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:36" x14ac:dyDescent="0.3">
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="K5" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="K5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="L5" s="22">
+      <c r="L5" s="35">
         <v>0.80208333333333337</v>
       </c>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21" t="s">
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21" t="s">
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21" t="s">
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="21"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5" s="34"/>
+      <c r="AE5" s="34"/>
       <c r="AH5" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AI5" s="7" t="s">
         <v>14</v>
@@ -1755,59 +1823,59 @@
         <v>17</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23" t="s">
+      <c r="L6" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23" t="s">
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23" t="s">
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23" t="s">
+      <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="33"/>
+      <c r="AA6" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB6" s="33"/>
+      <c r="AC6" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="23"/>
+      <c r="AD6" s="33"/>
+      <c r="AE6" s="33"/>
       <c r="AH6" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI6" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AI6" s="7" t="s">
+      <c r="AJ6" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="AJ6" s="8" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C7" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="28" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="7" t="s">
@@ -1817,57 +1885,57 @@
         <v>39</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23" t="s">
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23" t="s">
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
+      <c r="AA7" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB7" s="33"/>
+      <c r="AC7" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="23"/>
+      <c r="AD7" s="33"/>
+      <c r="AE7" s="33"/>
       <c r="AH7" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI7" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="AI7" s="7" t="s">
+      <c r="AJ7" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="AJ7" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="8" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C8" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="7" t="s">
         <v>35</v>
       </c>
@@ -1875,57 +1943,57 @@
         <v>40</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23" t="s">
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="33"/>
+      <c r="Z8" s="33"/>
+      <c r="AA8" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB8" s="33"/>
+      <c r="AC8" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
+      <c r="AD8" s="33"/>
+      <c r="AE8" s="33"/>
       <c r="AH8" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI8" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="AI8" s="7" t="s">
+      <c r="AJ8" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="AJ8" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="9" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="7" t="s">
         <v>36</v>
       </c>
@@ -1933,53 +2001,53 @@
         <v>41</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="31"/>
-      <c r="AA9" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB9" s="33"/>
+      <c r="AC9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="23"/>
+      <c r="AD9" s="33"/>
+      <c r="AE9" s="33"/>
       <c r="AH9" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI9" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="AI9" s="7" t="s">
+      <c r="AJ9" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="AJ9" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="10" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C10" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="7" t="s">
         <v>37</v>
       </c>
@@ -1987,78 +2055,78 @@
         <v>42</v>
       </c>
       <c r="AH10" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI10" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="AI10" s="7" t="s">
+      <c r="AJ10" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="AJ10" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="11" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C11" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E11" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="30" t="s">
         <v>35</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C12" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="19"/>
+        <v>129</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C13" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="20"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C14" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="30" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="7" t="s">
@@ -2070,13 +2138,13 @@
     </row>
     <row r="15" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C15" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="19"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="31"/>
       <c r="G15" s="7" t="s">
         <v>35</v>
       </c>
@@ -2086,13 +2154,13 @@
     </row>
     <row r="16" spans="3:36" x14ac:dyDescent="0.3">
       <c r="C16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="20"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="32"/>
       <c r="G16" s="7" t="s">
         <v>36</v>
       </c>
@@ -2102,15 +2170,15 @@
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="29" t="s">
         <v>37</v>
       </c>
       <c r="G17" s="7" t="s">
@@ -2122,13 +2190,13 @@
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
@@ -2138,15 +2206,15 @@
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="29" t="s">
         <v>38</v>
       </c>
       <c r="G19" s="7" t="s">
@@ -2158,13 +2226,13 @@
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="7" t="s">
         <v>35</v>
       </c>
@@ -2174,16 +2242,16 @@
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="27" t="s">
-        <v>131</v>
+      <c r="F21" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>34</v>
@@ -2194,34 +2262,34 @@
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="33"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="22"/>
       <c r="G22" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="32" t="s">
+      <c r="E23" s="26"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
@@ -2229,6 +2297,29 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="Q8:U8"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="V8:Z8"/>
+    <mergeCell ref="AC8:AE8"/>
+    <mergeCell ref="AC5:AE5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="V5:Z5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="L5:P5"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="V7:Z7"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="V6:Z6"/>
+    <mergeCell ref="AC9:AE9"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="L6:P6"/>
+    <mergeCell ref="AC7:AE7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="Q7:U7"/>
+    <mergeCell ref="L7:P7"/>
     <mergeCell ref="L9:Z9"/>
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="E21:E23"/>
@@ -2240,32 +2331,170 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="E11:E13"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="L6:P6"/>
-    <mergeCell ref="AC7:AE7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="Q7:U7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="V7:Z7"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="V6:Z6"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="F14:F16"/>
-    <mergeCell ref="AC5:AE5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="V5:Z5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="L5:P5"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="Q8:U8"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="V8:Z8"/>
-    <mergeCell ref="AC8:AE8"/>
-    <mergeCell ref="AC9:AE9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54182326-FFB7-4DB7-AEA3-42B4C432202E}">
+  <dimension ref="C5:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="6" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="25"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="25"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="25"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="25"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="25"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="25"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="26"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D9:D16"/>
+    <mergeCell ref="C9:C16"/>
+    <mergeCell ref="C5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D7:D16 F7:F16" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>